<commit_message>
improve creation of FE datasets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-methanol-heating.xlsx
+++ b/premise/data/additional_inventories/lci-methanol-heating.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09E06BB-AD21-AD41-91B5-0A48E133A037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861FF656-7DD0-5248-915C-D783DFA04374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34920" windowHeight="22720" xr2:uid="{56DD376B-3FB3-974E-BC88-AA42AC75F16A}"/>
+    <workbookView xWindow="2460" yWindow="2880" windowWidth="30240" windowHeight="18880" xr2:uid="{56DD376B-3FB3-974E-BC88-AA42AC75F16A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="93">
   <si>
     <t>Activity</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>methanol</t>
+  </si>
+  <si>
+    <t>methanol production, biomass gasification</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B5158D-BF09-CE4B-9D78-BA0E638D2994}">
   <dimension ref="A1:T112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2564,7 +2567,7 @@
     </row>
     <row r="76" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B76" s="7">
         <v>5.5555555555555601E-2</v>
@@ -2573,13 +2576,13 @@
         <v>8</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>43</v>
@@ -4042,5 +4045,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>